<commit_message>
test cases extended to add test for email validity and re-run after changes to css
</commit_message>
<xml_diff>
--- a/documentation/supp-spreadsheets/traceability matrix and test cases.xlsx
+++ b/documentation/supp-spreadsheets/traceability matrix and test cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>F01</t>
   </si>
@@ -299,6 +299,15 @@
 c. Tablet 768 x 1024 
 d. Larger tablet 1024 x 1366
 e. Smartphone 360 x 640</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>On the Contact page, attempt to Send message after entering a name and an invalid email address (i.e. email address that does not contain @)</t>
+  </si>
+  <si>
+    <t>User is prompted to enter a valid value in the email input field. Form is not submitted.</t>
   </si>
 </sst>
 </file>
@@ -462,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -474,6 +483,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,18 +516,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -504,16 +525,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -832,46 +844,46 @@
   <sheetData>
     <row r="2" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -897,7 +909,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -917,7 +929,7 @@
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -933,7 +945,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -949,7 +961,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
@@ -971,7 +983,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
@@ -989,7 +1001,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1019,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1034,346 +1046,373 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:F19"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A4:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="68.7109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="10" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="2" width="9.140625" style="12"/>
+    <col min="3" max="3" width="4.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="68.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="60.140625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:9" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="D4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="E4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="F4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="G4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="H4" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="D5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="E5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="F5" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="D6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="E6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="F6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="D7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="E7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="F7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="D8" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="E8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="F8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="D9" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="E9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="F9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="D10" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="E10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="F10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C11" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="D11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="E11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="F11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="G11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="D12" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="E12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="F12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="D13" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="E13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="F13" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="D14" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="E14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="F14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="G14" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="D15" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="E15" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="F15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="17" t="s">
+      <c r="G15" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="D16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="E17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="F17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="17" t="s">
+      <c r="G17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" s="11" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="17" t="s">
+    <row r="18" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="E18" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="F18" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="17" t="s">
+      <c r="G18" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="17" t="s">
+    <row r="19" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="E19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="F19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="17" t="s">
+      <c r="G19" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="17" t="s">
+    <row r="20" spans="3:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="C20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="E20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="F20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="G20" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="275" scale="67" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>